<commit_message>
Handling multiple DataProviders and suites
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/CustomerSuite.xlsx
+++ b/src/test/resources/testdata/CustomerSuite.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10875" windowHeight="8580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14925" windowHeight="6270"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TestCases" sheetId="1" r:id="rId1"/>
+    <sheet name="TestData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,6 +22,74 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+  <si>
+    <t>TestCases</t>
+  </si>
+  <si>
+    <t>RunMode</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>runMode</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>postalCode</t>
+  </si>
+  <si>
+    <t>Serge</t>
+  </si>
+  <si>
+    <t>Koko</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Dollar</t>
+  </si>
+  <si>
+    <t>Serge Koko</t>
+  </si>
+  <si>
+    <t>Harry Potter</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>EURO</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,12 +405,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>98125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Creating common utility for RunModes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/CustomerSuite.xlsx
+++ b/src/test/resources/testdata/CustomerSuite.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serge\eclipse-workspace\TestDataProject\src\test\resources\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14925" windowHeight="6270"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19395" windowHeight="10185" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="TestData" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:Q31"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -407,8 +403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +426,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -438,7 +434,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -450,7 +446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>